<commit_message>
Update files for IRD PCBv5
</commit_message>
<xml_diff>
--- a/PCBs/IRD_PCB_5/BOM_SMT_TB_RAK3172_868_IISS_PCB5.xlsx
+++ b/PCBs/IRD_PCB_5/BOM_SMT_TB_RAK3172_868_IISS_PCB5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cpham/Documents/TEX/Pau-05/PROJET-PRIMA-INTELIRRIS/PCBs/IRD-JFP/VRAK/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ECEDB28-EF29-5147-BA49-C43B3AE5516D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18F0F4C2-910B-0E48-9CAC-C609167BA374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4440" yWindow="780" windowWidth="24960" windowHeight="17280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1187,7 +1187,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1339,7 +1339,7 @@
         <v>9</v>
       </c>
       <c r="F6" t="s">
-        <v>22</v>
+        <v>92</v>
       </c>
       <c r="G6">
         <v>10.1</v>
@@ -1478,7 +1478,7 @@
         <v>9</v>
       </c>
       <c r="F11" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="G11">
         <v>5.5E-2</v>

</xml_diff>